<commit_message>
Skrip constraint mitnahmegewicht geadded projekt
</commit_message>
<xml_diff>
--- a/SAMPLE-Projektplanung.xlsx
+++ b/SAMPLE-Projektplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SQL-Kurs\Projekt\TierTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CAD367-5232-476A-9821-E84B319C0586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2466E896-5636-4F9C-BF41-08EAB7F3D28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="0" windowWidth="20490" windowHeight="11505" xr2:uid="{F9B33170-AAF7-4B35-BECE-784E17671F4A}"/>
+    <workbookView xWindow="1230" yWindow="270" windowWidth="18000" windowHeight="14205" xr2:uid="{F9B33170-AAF7-4B35-BECE-784E17671F4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Projekttasks" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="174">
   <si>
     <t>erledigt</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t>nicht bearbeitet stattdessen CURSOR erstellt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     als Muster Übungsaufgaben (Mietwagen) kann verwendet werden</t>
   </si>
   <si>
     <t>001-001</t>
@@ -582,13 +579,25 @@
     <t>Momentan Problem wenn mehrere Tier Verfügbar und eines Auftragsstatus 3</t>
   </si>
   <si>
-    <t xml:space="preserve">ein Trigger ( UPDATE ) Wenn endzeit eingefügt </t>
-  </si>
-  <si>
-    <t>ein Trigger ( UPDATE ) Wenn Rechnung erstellt</t>
-  </si>
-  <si>
     <t>005-002</t>
+  </si>
+  <si>
+    <t>While-Schleife</t>
+  </si>
+  <si>
+    <t>EXTRA</t>
+  </si>
+  <si>
+    <t>Mehr als eine Prozedur</t>
+  </si>
+  <si>
+    <t>ein Trigger Testscipt</t>
+  </si>
+  <si>
+    <t>ein Trigger ( UPDATE ) Wenn endzeit eingefügt  Logik im Skrip herausarbeiten</t>
+  </si>
+  <si>
+    <t>000-001</t>
   </si>
 </sst>
 </file>
@@ -763,7 +772,34 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1357,11 +1393,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5967EC-939C-45E1-A30B-BF7CDB6573C3}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1415,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1399,7 +1435,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>49</v>
@@ -1411,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="25" t="s">
@@ -1421,7 +1457,7 @@
         <v>27</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" s="6"/>
     </row>
@@ -1439,7 +1475,7 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1448,7 +1484,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>0</v>
@@ -1457,7 +1493,7 @@
         <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="8"/>
     </row>
@@ -1475,7 +1511,7 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="8"/>
     </row>
@@ -1487,13 +1523,13 @@
         <v>48</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H7" s="8"/>
     </row>
@@ -1502,7 +1538,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>0</v>
@@ -1511,7 +1547,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" s="8"/>
     </row>
@@ -1523,13 +1559,13 @@
         <v>30</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1595,7 +1631,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1637,7 +1673,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D18" t="s">
         <v>19</v>
@@ -1649,7 +1685,7 @@
         <v>27</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1661,7 +1697,7 @@
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>61</v>
@@ -1687,7 +1723,7 @@
         <v>27</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1704,7 +1740,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1718,13 +1754,13 @@
         <v>19</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F23" s="25" t="s">
         <v>27</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1732,7 +1768,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>0</v>
@@ -1741,7 +1777,7 @@
         <v>27</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1749,7 +1785,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="25"/>
@@ -1767,7 +1803,7 @@
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>76</v>
@@ -1841,7 +1877,7 @@
         <v>27</v>
       </c>
       <c r="G31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1849,327 +1885,388 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
         <v>166</v>
       </c>
-      <c r="E32" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" t="s">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>6</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>6</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="21" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="41" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="F34" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H34" s="21" t="s">
+      <c r="F44" s="21"/>
+      <c r="G44" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H44" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>8</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="23"/>
+      <c r="E47" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="23"/>
+      <c r="G47" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>9</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="22"/>
+      <c r="E51" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" t="s">
-        <v>79</v>
-      </c>
-      <c r="H35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>169</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-    </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" s="21" t="s">
+      <c r="F51" s="21"/>
+      <c r="G51" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H51" s="21" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="1">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="H43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>8</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="F45" s="23"/>
-      <c r="G45" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>38</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>9</v>
-      </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="H49" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>21</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" t="s">
-        <v>139</v>
-      </c>
-      <c r="H50" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" t="s">
+        <v>138</v>
+      </c>
+      <c r="H52" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+    <row r="58" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>10</v>
       </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="22" t="s">
+      <c r="B58" s="4"/>
+      <c r="C58" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="21" t="s">
+      <c r="D58" s="22"/>
+      <c r="E58" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="H56" s="21"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>40</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>81</v>
-      </c>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="H58" s="21"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C61" s="2" t="s">
+      <c r="E60" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E43 E21:F25">
-    <cfRule type="cellIs" dxfId="29" priority="67" operator="equal">
+  <conditionalFormatting sqref="E45 E21:F25">
+    <cfRule type="cellIs" dxfId="32" priority="70" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="71" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="72" operator="equal">
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
+  <conditionalFormatting sqref="E59">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+      <formula>"offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+      <formula>"erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:E49">
     <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2180,7 +2277,7 @@
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46:E47">
+  <conditionalFormatting sqref="E52:E53">
     <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2191,7 +2288,7 @@
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:E51">
+  <conditionalFormatting sqref="E42:F42">
     <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2202,7 +2299,7 @@
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40:F40">
+  <conditionalFormatting sqref="E37:F39">
     <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2213,7 +2310,7 @@
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35:F37">
+  <conditionalFormatting sqref="E29:F34">
     <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2224,18 +2321,18 @@
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:F32">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+  <conditionalFormatting sqref="E15:F18">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:F18">
+  <conditionalFormatting sqref="E12">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2246,7 +2343,7 @@
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E3:F9">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2257,7 +2354,7 @@
       <formula>"erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F9">
+  <conditionalFormatting sqref="E60">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"offen"</formula>
     </cfRule>
@@ -2277,7 +2374,7 @@
           <x14:formula1>
             <xm:f>Dropdownlisten!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E40:F40 E15:F18 E12 E57 E21:F25 E29:F32 E43 E50:E51 E46:E47 E3:F9 E35:F37</xm:sqref>
+          <xm:sqref>E42:F42 E15:F18 E12 E59 E21:F25 E37:F39 E45 E52:E53 E48:E49 E3:F9 E29:F34 E60</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2304,7 +2401,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2312,7 +2409,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>52</v>
@@ -2323,73 +2420,73 @@
     </row>
     <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="12"/>
     </row>
     <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D6" s="12"/>
     </row>
     <row r="7" spans="1:4" s="8" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" s="8" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D10" s="12"/>
     </row>
@@ -2427,7 +2524,7 @@
         <v>69</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>70</v>
@@ -2439,10 +2536,10 @@
         <v>71</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2451,34 +2548,34 @@
         <v>72</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>107</v>
-      </c>
       <c r="D16" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2492,78 +2589,78 @@
         <v>77</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>111</v>
-      </c>
       <c r="D19" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="12"/>
     </row>

</xml_diff>